<commit_message>
update description and rename step case column
</commit_message>
<xml_diff>
--- a/AnyX_Dashboard_test cases_KathieNgoanNguyen.xlsx
+++ b/AnyX_Dashboard_test cases_KathieNgoanNguyen.xlsx
@@ -11,22 +11,19 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="85">
   <si>
     <t>Description:</t>
   </si>
   <si>
-    <t xml:space="preserve">Purpose of this test to verify Dashboard Page Functionality
+    <t xml:space="preserve">Purpose of this test to verify Dashboard Page Functionalities
 </t>
   </si>
   <si>
-    <t>Objective: The objective of this test case is to verify the functionality of the dashboard page in terms of viewing data by publisher on a specific date range, viewing reports, creating cards, repositioning cards, removing cards within the Dashboard</t>
+    <t>Step number</t>
   </si>
   <si>
-    <t>Test case ID</t>
-  </si>
-  <si>
-    <t>Pass /Fail</t>
+    <t>Pass/Fail</t>
   </si>
   <si>
     <t>Step taken in AnyX</t>
@@ -56,7 +53,7 @@
         <i/>
         <color theme="1"/>
       </rPr>
-      <t>Login AnyX successfully with the Admin user role
+      <t>Login successfully
 There is at least 1 Publisher</t>
     </r>
     <r>
@@ -121,12 +118,11 @@
 ix. Custom</t>
   </si>
   <si>
-    <t xml:space="preserve">
-Select a time range in the dropdown list (from i to viii)</t>
+    <t>Select a Date range in the dropdown list (from i to viii)</t>
   </si>
   <si>
-    <t xml:space="preserve">- The Selected time range is showcased in the dropdown box. 
-- Data (for all cards in the dashboard) for that publisher in the selected time range are displayed </t>
+    <t xml:space="preserve">- The Selected Date range is showcased in the dropdown box. 
+- Data (for all cards in the dashboard) for that publisher in the selected Date range are displayed </t>
   </si>
   <si>
     <t>Re-click on the "Date Range" dropdown &gt; select "Custom"</t>
@@ -138,8 +134,8 @@
     <t>Select the start and end date from the calendar</t>
   </si>
   <si>
-    <t xml:space="preserve">- The Selected time range is showcased in the dropdown box. 
-- Data (for all cards in the dashboard) for that publisher in the selected time range are updated and displayed </t>
+    <t xml:space="preserve">- The Selected Date range is showcased in the dropdown box. 
+- Data (for all cards in the dashboard) for that publisher in the selected Date range are updated and displayed </t>
   </si>
   <si>
     <t>Click on the "Refresh Data" button on the header panel</t>
@@ -254,7 +250,7 @@
   </si>
   <si>
     <t>- The new selected Publisher name and Date range are updated in the corresponding dropdown boxes on the header panel 
--The Summary cards for the selected time range of the Publisher is created on the dashboard contains information:
+-The Summary cards for the selected Date range of the Publisher is created on the dashboard contains information:
 a. Requests
 b. Impressions
 c. Clicks
@@ -311,7 +307,7 @@
 * Chart type
 * Color of the chart
 * Metric report
-* Time range</t>
+* Date range</t>
   </si>
   <si>
     <t>The left chart: Click on the remaining "Metric dropdown"</t>
@@ -354,7 +350,7 @@
 - The chart is created with correct information:
 * Chart type
 * Metric report
-* Time range</t>
+* Date range</t>
   </si>
   <si>
     <t xml:space="preserve">Click on the "View Report" button in the Graph card </t>
@@ -1122,9 +1118,7 @@
       <c r="Z4" s="1"/>
     </row>
     <row r="5">
-      <c r="A5" s="5" t="s">
-        <v>2</v>
-      </c>
+      <c r="A5" s="5"/>
       <c r="G5" s="6"/>
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
@@ -1176,22 +1170,22 @@
     </row>
     <row r="7">
       <c r="A7" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="C7" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="D7" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="E7" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="E7" s="7" t="s">
+      <c r="F7" s="7" t="s">
         <v>7</v>
-      </c>
-      <c r="F7" s="7" t="s">
-        <v>8</v>
       </c>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
@@ -1220,14 +1214,14 @@
       </c>
       <c r="B8" s="8"/>
       <c r="C8" s="8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E8" s="9"/>
       <c r="F8" s="8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
@@ -1256,10 +1250,10 @@
       </c>
       <c r="B9" s="8"/>
       <c r="C9" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E9" s="10"/>
       <c r="F9" s="9"/>
@@ -1290,10 +1284,10 @@
       </c>
       <c r="B10" s="8"/>
       <c r="C10" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E10" s="9"/>
       <c r="F10" s="9"/>
@@ -1324,10 +1318,10 @@
       </c>
       <c r="B11" s="8"/>
       <c r="C11" s="8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E11" s="9"/>
       <c r="F11" s="9"/>
@@ -1358,10 +1352,10 @@
       </c>
       <c r="B12" s="8"/>
       <c r="C12" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E12" s="9"/>
       <c r="F12" s="9"/>
@@ -1392,10 +1386,10 @@
       </c>
       <c r="B13" s="8"/>
       <c r="C13" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E13" s="9"/>
       <c r="F13" s="9"/>
@@ -1426,10 +1420,10 @@
       </c>
       <c r="B14" s="8"/>
       <c r="C14" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E14" s="9"/>
       <c r="F14" s="9"/>
@@ -1460,10 +1454,10 @@
       </c>
       <c r="B15" s="8"/>
       <c r="C15" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E15" s="9"/>
       <c r="F15" s="9"/>
@@ -1494,14 +1488,14 @@
       </c>
       <c r="B16" s="8"/>
       <c r="C16" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E16" s="10"/>
       <c r="F16" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
@@ -1530,10 +1524,10 @@
       </c>
       <c r="B17" s="8"/>
       <c r="C17" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E17" s="9"/>
       <c r="F17" s="9"/>
@@ -1564,10 +1558,10 @@
       </c>
       <c r="B18" s="8"/>
       <c r="C18" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E18" s="9"/>
       <c r="F18" s="9"/>
@@ -1598,10 +1592,10 @@
       </c>
       <c r="B19" s="8"/>
       <c r="C19" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E19" s="9"/>
       <c r="F19" s="8"/>
@@ -1632,10 +1626,10 @@
       </c>
       <c r="B20" s="8"/>
       <c r="C20" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E20" s="9"/>
       <c r="F20" s="8"/>
@@ -1666,10 +1660,10 @@
       </c>
       <c r="B21" s="8"/>
       <c r="C21" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D21" s="11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E21" s="9"/>
       <c r="F21" s="8"/>
@@ -1700,10 +1694,10 @@
       </c>
       <c r="B22" s="8"/>
       <c r="C22" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E22" s="9"/>
       <c r="F22" s="8"/>
@@ -1734,10 +1728,10 @@
       </c>
       <c r="B23" s="8"/>
       <c r="C23" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E23" s="9"/>
       <c r="F23" s="8"/>
@@ -1768,10 +1762,10 @@
       </c>
       <c r="B24" s="8"/>
       <c r="C24" s="8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D24" s="12" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E24" s="9"/>
       <c r="F24" s="8"/>
@@ -1802,10 +1796,10 @@
       </c>
       <c r="B25" s="8"/>
       <c r="C25" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E25" s="9"/>
       <c r="F25" s="8"/>
@@ -1836,10 +1830,10 @@
       </c>
       <c r="B26" s="8"/>
       <c r="C26" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E26" s="9"/>
       <c r="F26" s="8"/>
@@ -1870,10 +1864,10 @@
       </c>
       <c r="B27" s="8"/>
       <c r="C27" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E27" s="9"/>
       <c r="F27" s="8"/>
@@ -1904,10 +1898,10 @@
       </c>
       <c r="B28" s="8"/>
       <c r="C28" s="13" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D28" s="12" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E28" s="9"/>
       <c r="F28" s="8"/>
@@ -1938,10 +1932,10 @@
       </c>
       <c r="B29" s="8"/>
       <c r="C29" s="13" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E29" s="9"/>
       <c r="F29" s="8"/>
@@ -1972,10 +1966,10 @@
       </c>
       <c r="B30" s="8"/>
       <c r="C30" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E30" s="9"/>
       <c r="F30" s="8"/>
@@ -2006,10 +2000,10 @@
       </c>
       <c r="B31" s="8"/>
       <c r="C31" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D31" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E31" s="9"/>
       <c r="F31" s="8"/>
@@ -2040,10 +2034,10 @@
       </c>
       <c r="B32" s="8"/>
       <c r="C32" s="8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D32" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E32" s="9"/>
       <c r="F32" s="8"/>
@@ -2074,10 +2068,10 @@
       </c>
       <c r="B33" s="8"/>
       <c r="C33" s="8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D33" s="8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E33" s="9"/>
       <c r="F33" s="8"/>
@@ -2108,10 +2102,10 @@
       </c>
       <c r="B34" s="8"/>
       <c r="C34" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E34" s="9"/>
       <c r="F34" s="8"/>
@@ -2142,10 +2136,10 @@
       </c>
       <c r="B35" s="8"/>
       <c r="C35" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D35" s="8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E35" s="9"/>
       <c r="F35" s="8"/>
@@ -2176,10 +2170,10 @@
       </c>
       <c r="B36" s="8"/>
       <c r="C36" s="8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D36" s="8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E36" s="9"/>
       <c r="F36" s="8"/>
@@ -2210,10 +2204,10 @@
       </c>
       <c r="B37" s="8"/>
       <c r="C37" s="8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D37" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E37" s="9"/>
       <c r="F37" s="8"/>
@@ -2244,10 +2238,10 @@
       </c>
       <c r="B38" s="8"/>
       <c r="C38" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D38" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E38" s="9"/>
       <c r="F38" s="8"/>
@@ -2278,10 +2272,10 @@
       </c>
       <c r="B39" s="8"/>
       <c r="C39" s="8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D39" s="8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E39" s="9"/>
       <c r="F39" s="8"/>
@@ -2312,10 +2306,10 @@
       </c>
       <c r="B40" s="8"/>
       <c r="C40" s="8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D40" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E40" s="9"/>
       <c r="F40" s="9"/>
@@ -2346,10 +2340,10 @@
       </c>
       <c r="B41" s="8"/>
       <c r="C41" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D41" s="8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E41" s="9"/>
       <c r="F41" s="9"/>
@@ -2380,10 +2374,10 @@
       </c>
       <c r="B42" s="8"/>
       <c r="C42" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D42" s="8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E42" s="9"/>
       <c r="F42" s="9"/>
@@ -2414,10 +2408,10 @@
       </c>
       <c r="B43" s="8"/>
       <c r="C43" s="8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D43" s="8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E43" s="9"/>
       <c r="F43" s="9"/>
@@ -2448,10 +2442,10 @@
       </c>
       <c r="B44" s="8"/>
       <c r="C44" s="8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D44" s="8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E44" s="9"/>
       <c r="F44" s="9"/>
@@ -2506,7 +2500,7 @@
     </row>
     <row r="46">
       <c r="A46" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
@@ -2536,7 +2530,7 @@
     </row>
     <row r="47">
       <c r="A47" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
@@ -2566,7 +2560,7 @@
     </row>
     <row r="48">
       <c r="A48" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
@@ -2652,7 +2646,7 @@
     </row>
     <row r="51">
       <c r="A51" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
@@ -2682,7 +2676,7 @@
     </row>
     <row r="52">
       <c r="A52" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
@@ -2712,7 +2706,7 @@
     </row>
     <row r="53">
       <c r="A53" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>

</xml_diff>